<commit_message>
GitHub Action: generate latest manifests
</commit_message>
<xml_diff>
--- a/current-excel-manifests/Assay16SrRNAseqMetadataTemplate.xlsx
+++ b/current-excel-manifests/Assay16SrRNAseqMetadataTemplate.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="346">
   <si>
     <t>Component</t>
   </si>
@@ -519,574 +519,586 @@
     <t>H3K36me3</t>
   </si>
   <si>
+    <t>Illumina EPIC Array</t>
+  </si>
+  <si>
+    <t>IlluminaInfiniumGSAMD-24v2-0</t>
+  </si>
+  <si>
+    <t>H3K4me1</t>
+  </si>
+  <si>
     <t>Immunocytochemistry</t>
   </si>
   <si>
-    <t>IlluminaInfiniumGSAMD-24v2-0</t>
-  </si>
-  <si>
-    <t>H3K4me1</t>
+    <t>IlluminaMethylationEPIC</t>
+  </si>
+  <si>
+    <t>H3K4me3</t>
   </si>
   <si>
     <t>immunofluorescence</t>
   </si>
   <si>
-    <t>IlluminaMethylationEPIC</t>
-  </si>
-  <si>
-    <t>H3K4me3</t>
+    <t>IlluminaMiSeq</t>
+  </si>
+  <si>
+    <t>H3K9ac</t>
   </si>
   <si>
     <t>immunohistochemistry</t>
   </si>
   <si>
-    <t>IlluminaMiSeq</t>
-  </si>
-  <si>
-    <t>H3K9ac</t>
+    <t>IlluminaNovaseq6000</t>
+  </si>
+  <si>
+    <t>H3K9me2</t>
   </si>
   <si>
     <t>in vivo bioluminescence</t>
   </si>
   <si>
-    <t>IlluminaNovaseq6000</t>
-  </si>
-  <si>
-    <t>H3K9me2</t>
+    <t>IlluminaWholeGenomeDASL</t>
+  </si>
+  <si>
+    <t>H3K9me3</t>
   </si>
   <si>
     <t>ISOSeq</t>
   </si>
   <si>
-    <t>IlluminaWholeGenomeDASL</t>
-  </si>
-  <si>
-    <t>H3K9me3</t>
+    <t>Infinium Global Diversity Array-8</t>
+  </si>
+  <si>
+    <t>HCFC1</t>
   </si>
   <si>
     <t>jumpingLibrary</t>
   </si>
   <si>
-    <t>Infinium Global Diversity Array-8</t>
-  </si>
-  <si>
-    <t>HCFC1</t>
+    <t>Infinium HumanOmniExpressExome</t>
+  </si>
+  <si>
+    <t>HNRNPK</t>
   </si>
   <si>
     <t>kinesthetic behavior</t>
   </si>
   <si>
-    <t>Infinium HumanOmniExpressExome</t>
-  </si>
-  <si>
-    <t>HNRNPK</t>
+    <t>Infinium Omni2.5Exome-8 v1.1</t>
+  </si>
+  <si>
+    <t>IE_V1-V3</t>
   </si>
   <si>
     <t>label free mass spectrometry</t>
   </si>
   <si>
-    <t>Infinium Omni2.5Exome-8 v1.1</t>
-  </si>
-  <si>
-    <t>IE_V1-V3</t>
+    <t>Infinium Omni2.5Exome-8 v1.3</t>
+  </si>
+  <si>
+    <t>IgG</t>
   </si>
   <si>
     <t>Laser Speckle Imaging</t>
   </si>
   <si>
-    <t>Infinium Omni2.5Exome-8 v1.3</t>
-  </si>
-  <si>
-    <t>IgG</t>
+    <t>Infinium Omni2.5Exome-8 v1.4</t>
+  </si>
+  <si>
+    <t>input</t>
   </si>
   <si>
     <t>LC-MS</t>
   </si>
   <si>
-    <t>Infinium Omni2.5Exome-8 v1.4</t>
-  </si>
-  <si>
-    <t>input</t>
+    <t>Infinium Omni2.5Exome-8 v1.5</t>
+  </si>
+  <si>
+    <t>KAT2B</t>
   </si>
   <si>
     <t>LC-MSMS</t>
   </si>
   <si>
-    <t>Infinium Omni2.5Exome-8 v1.5</t>
-  </si>
-  <si>
-    <t>KAT2B</t>
+    <t>InfiniumPsychArrayBeadChip</t>
+  </si>
+  <si>
+    <t>KDM4A</t>
   </si>
   <si>
     <t>LC-SRM</t>
   </si>
   <si>
-    <t>InfiniumPsychArrayBeadChip</t>
-  </si>
-  <si>
-    <t>KDM4A</t>
+    <t>Leco Pegasus IV</t>
+  </si>
+  <si>
+    <t>KLF16</t>
   </si>
   <si>
     <t>Leiden Oxylipins</t>
   </si>
   <si>
-    <t>Leco Pegasus IV</t>
-  </si>
-  <si>
-    <t>KLF16</t>
+    <t>llumina Infinium General Screening Array 24-Kit v3.0</t>
+  </si>
+  <si>
+    <t>KLF5</t>
   </si>
   <si>
     <t>lentiMPRA</t>
   </si>
   <si>
-    <t>llumina Infinium General Screening Array 24-Kit v3.0</t>
-  </si>
-  <si>
-    <t>KLF5</t>
+    <t>LTQOrbitrapXL</t>
+  </si>
+  <si>
+    <t>LaminB</t>
   </si>
   <si>
     <t>LFP</t>
   </si>
   <si>
-    <t>LTQOrbitrapXL</t>
-  </si>
-  <si>
-    <t>LaminB</t>
+    <t>MiSeq</t>
+  </si>
+  <si>
+    <t>MAZ</t>
   </si>
   <si>
     <t>liquid chromatography-electrochemical detection</t>
   </si>
   <si>
-    <t>MiSeq</t>
-  </si>
-  <si>
-    <t>MAZ</t>
+    <t>NanostringnCounter</t>
+  </si>
+  <si>
+    <t>MEF2A</t>
   </si>
   <si>
     <t>lncrnaSeq</t>
   </si>
   <si>
-    <t>NanostringnCounter</t>
-  </si>
-  <si>
-    <t>MEF2A</t>
+    <t>NanostringnCounter_MouseADPanel</t>
+  </si>
+  <si>
+    <t>MEIS2</t>
   </si>
   <si>
     <t>locomotor activation behavior</t>
   </si>
   <si>
-    <t>NanostringnCounter_MouseADPanel</t>
-  </si>
-  <si>
-    <t>MEIS2</t>
+    <t>NextSeq2000</t>
+  </si>
+  <si>
+    <t>MITF</t>
   </si>
   <si>
     <t>long-read rnaSeq</t>
   </si>
   <si>
-    <t>NextSeq2000</t>
-  </si>
-  <si>
-    <t>MITF</t>
+    <t>NextSeq500</t>
+  </si>
+  <si>
+    <t>NCOA2</t>
   </si>
   <si>
     <t>LTP</t>
   </si>
   <si>
-    <t>NextSeq500</t>
-  </si>
-  <si>
-    <t>NCOA2</t>
+    <t>Olink Target 96</t>
+  </si>
+  <si>
+    <t>NCOR1</t>
   </si>
   <si>
     <t>m6A-rnaSeq</t>
   </si>
   <si>
-    <t>Olink Target 96</t>
-  </si>
-  <si>
-    <t>NCOR1</t>
+    <t>orbitrap</t>
+  </si>
+  <si>
+    <t>NEUROD1</t>
   </si>
   <si>
     <t>MDMS-SL</t>
   </si>
   <si>
-    <t>orbitrap</t>
-  </si>
-  <si>
-    <t>NEUROD1</t>
+    <t>Orbitrap Exploris 240</t>
+  </si>
+  <si>
+    <t>NFIB</t>
   </si>
   <si>
     <t>memory behavior</t>
   </si>
   <si>
-    <t>Orbitrap Exploris 240</t>
-  </si>
-  <si>
-    <t>NFIB</t>
+    <t>OrbiTrap Fusion</t>
+  </si>
+  <si>
+    <t>NFIC</t>
   </si>
   <si>
     <t>Metabolon</t>
   </si>
   <si>
-    <t>OrbiTrap Fusion</t>
-  </si>
-  <si>
-    <t>NFIC</t>
+    <t>Orbitrap Fusion Lumos</t>
+  </si>
+  <si>
+    <t>NONO</t>
   </si>
   <si>
     <t>methylationArray</t>
   </si>
   <si>
-    <t>Orbitrap Fusion Lumos</t>
-  </si>
-  <si>
-    <t>NONO</t>
+    <t>PacBio Sequel II</t>
+  </si>
+  <si>
+    <t>NR2F1</t>
   </si>
   <si>
     <t>MIB/MS</t>
   </si>
   <si>
-    <t>PacBio Sequel II</t>
-  </si>
-  <si>
-    <t>NR2F1</t>
+    <t>PacBio Sequel IIe</t>
+  </si>
+  <si>
+    <t>NR2F2</t>
   </si>
   <si>
     <t>microRNAcounts</t>
   </si>
   <si>
-    <t>PacBio Sequel IIe</t>
-  </si>
-  <si>
-    <t>NR2F2</t>
+    <t>PacBioRSII</t>
+  </si>
+  <si>
+    <t>NR3C1</t>
   </si>
   <si>
     <t>mirnaArray</t>
   </si>
   <si>
-    <t>PacBioRSII</t>
-  </si>
-  <si>
-    <t>NR3C1</t>
+    <t>Perlegen300Karray</t>
+  </si>
+  <si>
+    <t>NRF1</t>
   </si>
   <si>
     <t>mirnaSeq</t>
   </si>
   <si>
-    <t>Perlegen300Karray</t>
-  </si>
-  <si>
-    <t>NRF1</t>
+    <t>PsychChip</t>
+  </si>
+  <si>
+    <t>OLIG2</t>
   </si>
   <si>
     <t>MRI</t>
   </si>
   <si>
-    <t>PsychChip</t>
-  </si>
-  <si>
-    <t>OLIG2</t>
+    <t>Q Exactive</t>
+  </si>
+  <si>
+    <t>PKNOX1</t>
   </si>
   <si>
     <t>mRNAcounts</t>
   </si>
   <si>
-    <t>Q Exactive</t>
-  </si>
-  <si>
-    <t>PKNOX1</t>
+    <t>Q Exactive HF</t>
+  </si>
+  <si>
+    <t>Pol2</t>
+  </si>
+  <si>
+    <t>mRNAseq</t>
+  </si>
+  <si>
+    <t>Q Exactive HF-X</t>
+  </si>
+  <si>
+    <t>R-loops</t>
   </si>
   <si>
     <t>MudPIT</t>
   </si>
   <si>
-    <t>Q Exactive HF</t>
-  </si>
-  <si>
-    <t>Pol2</t>
+    <t>Q Exactive Plus</t>
+  </si>
+  <si>
+    <t>RAD21</t>
   </si>
   <si>
     <t>nextGenerationTargetedSequencing</t>
   </si>
   <si>
-    <t>Q Exactive HF-X</t>
-  </si>
-  <si>
-    <t>R-loops</t>
+    <t>quadrupole time-of-flight</t>
+  </si>
+  <si>
+    <t>RB1</t>
   </si>
   <si>
     <t>Nightingale NMR</t>
   </si>
   <si>
-    <t>Q Exactive Plus</t>
-  </si>
-  <si>
-    <t>RAD21</t>
+    <t>Roche Cobas</t>
+  </si>
+  <si>
+    <t>RELB</t>
   </si>
   <si>
     <t>NOMe-Seq</t>
   </si>
   <si>
-    <t>quadrupole time-of-flight</t>
-  </si>
-  <si>
-    <t>RB1</t>
+    <t>SequenomMultiplex</t>
+  </si>
+  <si>
+    <t>REST</t>
   </si>
   <si>
     <t>novelty response behavior</t>
   </si>
   <si>
-    <t>Roche Cobas</t>
-  </si>
-  <si>
-    <t>RELB</t>
+    <t>Signa Premier AIR 3T</t>
+  </si>
+  <si>
+    <t>SATB2</t>
   </si>
   <si>
     <t>open field test</t>
   </si>
   <si>
-    <t>SequenomMultiplex</t>
-  </si>
-  <si>
-    <t>REST</t>
+    <t>Simoa HD-1 Analyzer</t>
+  </si>
+  <si>
+    <t>SIN3A</t>
   </si>
   <si>
     <t>oxBS-Seq</t>
   </si>
   <si>
-    <t>Signa Premier AIR 3T</t>
-  </si>
-  <si>
-    <t>SATB2</t>
+    <t>time-of-flight</t>
+  </si>
+  <si>
+    <t>SIN3B</t>
   </si>
   <si>
     <t>pharmacodynamics</t>
   </si>
   <si>
-    <t>Simoa HD-1 Analyzer</t>
-  </si>
-  <si>
-    <t>SIN3A</t>
+    <t>triple quadrupole</t>
+  </si>
+  <si>
+    <t>SIRT1</t>
   </si>
   <si>
     <t>pharmacokinetics</t>
   </si>
   <si>
-    <t>time-of-flight</t>
-  </si>
-  <si>
-    <t>SIN3B</t>
+    <t>Xevo G2 QTOF</t>
+  </si>
+  <si>
+    <t>SIX4</t>
   </si>
   <si>
     <t>photograph</t>
   </si>
   <si>
-    <t>triple quadrupole</t>
-  </si>
-  <si>
-    <t>SIRT1</t>
+    <t>Xevo TQ-S</t>
+  </si>
+  <si>
+    <t>SKIL</t>
   </si>
   <si>
     <t>polymeraseChainReaction</t>
   </si>
   <si>
-    <t>Xevo G2 QTOF</t>
-  </si>
-  <si>
-    <t>SIX4</t>
+    <t>SMARCA5</t>
   </si>
   <si>
     <t>Positron Emission Tomography</t>
   </si>
   <si>
-    <t>Xevo TQ-S</t>
-  </si>
-  <si>
-    <t>SKIL</t>
+    <t>SMC3</t>
   </si>
   <si>
     <t>proximity extension assay</t>
   </si>
   <si>
-    <t>SMARCA5</t>
+    <t>SON</t>
   </si>
   <si>
     <t>questionnaire</t>
   </si>
   <si>
-    <t>SMC3</t>
+    <t>SOX8</t>
   </si>
   <si>
     <t>Rader Lipidomics</t>
   </si>
   <si>
-    <t>SON</t>
+    <t>SP1</t>
   </si>
   <si>
     <t>Real Time PCR</t>
   </si>
   <si>
-    <t>SOX8</t>
+    <t>SP4</t>
   </si>
   <si>
     <t>Ribo-Seq</t>
   </si>
   <si>
-    <t>SP1</t>
+    <t>SREBP2</t>
   </si>
   <si>
     <t>rnaArray</t>
   </si>
   <si>
-    <t>SP4</t>
+    <t>SRF</t>
   </si>
   <si>
     <t>rnaSeq</t>
   </si>
   <si>
-    <t>SREBP2</t>
+    <t>TAF1</t>
   </si>
   <si>
     <t>rotarod performance test</t>
   </si>
   <si>
-    <t>SRF</t>
+    <t>TBR1</t>
   </si>
   <si>
     <t>RPPA</t>
   </si>
   <si>
-    <t>TAF1</t>
+    <t>TCF12</t>
+  </si>
+  <si>
+    <t>RRBS</t>
+  </si>
+  <si>
+    <t>TCF7L2</t>
   </si>
   <si>
     <t>sandwich ELISA</t>
   </si>
   <si>
-    <t>TBR1</t>
+    <t>TDP43</t>
   </si>
   <si>
     <t>Sanger sequencing</t>
   </si>
   <si>
-    <t>TCF12</t>
+    <t>TRIM28</t>
   </si>
   <si>
     <t>scale</t>
   </si>
   <si>
-    <t>TCF7L2</t>
+    <t>YBX1</t>
   </si>
   <si>
     <t>scATACSeq</t>
   </si>
   <si>
-    <t>TDP43</t>
+    <t>YBX3</t>
   </si>
   <si>
     <t>scCGIseq</t>
   </si>
   <si>
-    <t>TRIM28</t>
+    <t>YY1</t>
   </si>
   <si>
     <t>scirnaSeq</t>
   </si>
   <si>
-    <t>YBX1</t>
+    <t>ZBTB7B</t>
   </si>
   <si>
     <t>scrnaSeq</t>
   </si>
   <si>
-    <t>YBX3</t>
+    <t>ZEB1</t>
   </si>
   <si>
     <t>scwholeGenomeSeq</t>
   </si>
   <si>
-    <t>YY1</t>
+    <t>ZEB2</t>
   </si>
   <si>
     <t>SiMoA</t>
   </si>
   <si>
-    <t>ZBTB7B</t>
+    <t>ZFP91</t>
   </si>
   <si>
     <t>snATACSeq</t>
   </si>
   <si>
-    <t>ZEB1</t>
+    <t>ZHX1</t>
   </si>
   <si>
     <t>snpArray</t>
   </si>
   <si>
-    <t>ZEB2</t>
+    <t>ZKSCAN1</t>
   </si>
   <si>
     <t>snrnaSeq</t>
   </si>
   <si>
-    <t>ZFP91</t>
+    <t>ZNF143</t>
   </si>
   <si>
     <t>spontaneous alternation</t>
   </si>
   <si>
-    <t>ZHX1</t>
-  </si>
-  <si>
-    <t>ZKSCAN1</t>
+    <t>ZNF207</t>
+  </si>
+  <si>
+    <t>ZNF24</t>
   </si>
   <si>
     <t>TMT quantitation</t>
   </si>
   <si>
-    <t>ZNF143</t>
+    <t>ZNF318</t>
+  </si>
+  <si>
+    <t>TotalRNAseq</t>
+  </si>
+  <si>
+    <t>ZNF384</t>
   </si>
   <si>
     <t>tractionForceMicroscopy</t>
   </si>
   <si>
-    <t>ZNF207</t>
+    <t>ZNF407</t>
   </si>
   <si>
     <t>UC Davis GCTOF</t>
   </si>
   <si>
-    <t>ZNF24</t>
+    <t>ZNF592</t>
   </si>
   <si>
     <t>UCSD Untargeted Metabolomics</t>
   </si>
   <si>
-    <t>ZNF318</t>
+    <t>ZSCAN29</t>
   </si>
   <si>
     <t>UPLC-ESI-QTOF-MS</t>
   </si>
   <si>
-    <t>ZNF384</t>
-  </si>
-  <si>
     <t>UPLC-MSMS</t>
   </si>
   <si>
-    <t>ZNF407</t>
-  </si>
-  <si>
     <t>Vernier Caliper</t>
   </si>
   <si>
-    <t>ZNF592</t>
-  </si>
-  <si>
     <t>von Frey test</t>
-  </si>
-  <si>
-    <t>ZSCAN29</t>
   </si>
   <si>
     <t>westernBlot</t>
@@ -28466,11 +28478,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="D2:D1000">
       <formula1>Sheet2!$D$2:$D$81</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="C2:C1000">
+      <formula1>Sheet2!$C$2:$C$123</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="I2:I1000">
       <formula1>Sheet2!$I$2:$I$21</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="C2:C1000">
-      <formula1>Sheet2!$C$2:$C$119</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Choose one from dropdown" sqref="L2:L1000">
       <formula1>Sheet2!$L$2:$L$112</formula1>
@@ -29653,31 +29665,31 @@
     </row>
     <row r="104">
       <c r="C104" s="7" t="s">
-        <v>84</v>
+        <v>318</v>
       </c>
       <c r="L104" s="7" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="105">
       <c r="C105" s="7" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="L105" s="7" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="106">
       <c r="C106" s="7" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L106" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="107">
       <c r="C107" s="7" t="s">
-        <v>323</v>
+        <v>84</v>
       </c>
       <c r="L107" s="7" t="s">
         <v>324</v>
@@ -29756,6 +29768,26 @@
     <row r="119">
       <c r="C119" s="7" t="s">
         <v>341</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="C120" s="7" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="C121" s="7" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="C122" s="7" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="C123" s="7" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>

</xml_diff>